<commit_message>
actualización solicitgrafica de recursos 10-02
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/EscaletaCN_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/EscaletaCN_10_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PLANETA 10 Y 11\CN_10_02_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\CienciasNaturales\fuentes\contenidos\grado10\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -778,7 +778,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,6 +848,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,7 +1017,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1189,18 +1195,36 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1240,22 +1264,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1649,7 +1661,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,94 +1690,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="L1" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="75" t="s">
+      <c r="M1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="63" t="s">
+      <c r="N1" s="81"/>
+      <c r="O1" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="63" t="s">
+      <c r="P1" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="Q1" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="82" t="s">
+      <c r="R1" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="78" t="s">
+      <c r="S1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="80" t="s">
+      <c r="T1" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="78" t="s">
+      <c r="U1" s="63" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="70"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="35" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="79"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="64"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1785,7 +1797,7 @@
       <c r="G3" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="84">
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
@@ -1907,7 +1919,7 @@
       <c r="G5" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="84">
         <v>3</v>
       </c>
       <c r="I5" s="13" t="s">
@@ -2206,7 +2218,7 @@
       <c r="G10" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="85">
         <v>8</v>
       </c>
       <c r="I10" s="30" t="s">
@@ -2501,7 +2513,7 @@
       <c r="G15" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="84">
         <v>13</v>
       </c>
       <c r="I15" s="30" t="s">
@@ -3354,7 +3366,7 @@
       <c r="G30" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="84">
         <v>28</v>
       </c>
       <c r="I30" s="30" t="s">
@@ -4580,12 +4592,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4600,6 +4606,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>